<commit_message>
el corrector del frame se incorporo al programa
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/A completar/Excel 397 - copia (3) - copia.xlsx
+++ b/Archivos de trabajo/A completar/Excel 397 - copia (3) - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Emma\14. Vulcano\RelojRRHH\Proyecto\Archivos de trabajo\A completar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC429ED-60E5-4D26-90B7-96A3AEE3832D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C915DC1D-C442-45E0-9559-D51D8664B4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,9 +113,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -176,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -189,6 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,10 +585,10 @@
       <c r="D2" s="2">
         <v>44186</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="10">
         <v>44186.311111111107</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="10">
         <v>44186.836111111108</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -638,10 +640,10 @@
       <c r="D3" s="2">
         <v>44187</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="10">
         <v>44187.315972222219</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="10">
         <v>44187.834722222222</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -693,10 +695,10 @@
       <c r="D4" s="2">
         <v>44188</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="10">
         <v>44188.314583333333</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="10">
         <v>44188.834027777782</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -748,10 +750,10 @@
       <c r="D5" s="2">
         <v>44189</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="10">
         <v>44189.333333333343</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="10">
         <v>44189.499305555553</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -803,10 +805,10 @@
       <c r="D6" s="5">
         <v>44190</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="10">
         <v>44190</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="10">
         <v>44190</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -858,10 +860,10 @@
       <c r="D7" s="5">
         <v>44191</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="10">
         <v>44191</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="10">
         <v>44191</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -913,10 +915,10 @@
       <c r="D8" s="5">
         <v>44192</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="10">
         <v>44192</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="10">
         <v>44192</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -968,10 +970,10 @@
       <c r="D9" s="8">
         <v>44194</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="10">
         <v>44193.809027777781</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="10">
         <v>44194.334722222222</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -1023,10 +1025,10 @@
       <c r="D10" s="8">
         <v>44195</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="10">
         <v>44194.80972222222</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="10">
         <v>44195.334027777782</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1078,10 +1080,10 @@
       <c r="D11" s="8">
         <v>44196</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="10">
         <v>44195.801388888889</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="10">
         <v>44196.334027777782</v>
       </c>
       <c r="G11" s="9"/>
@@ -1117,10 +1119,10 @@
       <c r="D12" s="5">
         <v>44197</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="10">
         <v>44197</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="10">
         <v>44197</v>
       </c>
       <c r="G12" s="6"/>
@@ -1156,10 +1158,10 @@
       <c r="D13" s="5">
         <v>44198</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="10">
         <v>44198</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="10">
         <v>44198</v>
       </c>
       <c r="G13" s="6"/>

</xml_diff>